<commit_message>
update to output excel file
</commit_message>
<xml_diff>
--- a/data/Test-Data.xlsx
+++ b/data/Test-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/913814a93b0a3fc4/Documents/002 Projects/002 Freelance/1 - Javier Gutierrez/Scraper00/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_F25DC773A252ABDACC1048EA11DB478C5BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AA833B1-4269-47C1-80C3-A7AACA707ABC}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_F25DC773A252ABDACC1048EA11DB478C5BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B75EE83-2DE0-433C-A4F1-F6CF3C6056B7}"/>
   <bookViews>
-    <workbookView xWindow="2184" yWindow="4632" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24765" yWindow="2475" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Company</t>
   </si>
@@ -85,96 +85,6 @@
   </si>
   <si>
     <t>www.sfermion.io</t>
-  </si>
-  <si>
-    <t>NGN Capital</t>
-  </si>
-  <si>
-    <t>www.ngncapital.com</t>
-  </si>
-  <si>
-    <t>LRI</t>
-  </si>
-  <si>
-    <t>www.unlockvp.com</t>
-  </si>
-  <si>
-    <t>Invus</t>
-  </si>
-  <si>
-    <t>www.invus.com</t>
-  </si>
-  <si>
-    <t>Trinity Ventures</t>
-  </si>
-  <si>
-    <t>www.trinityventures.com</t>
-  </si>
-  <si>
-    <t>Hatteras Venture Partners</t>
-  </si>
-  <si>
-    <t>www.hatterasvp.com</t>
-  </si>
-  <si>
-    <t>Brightstone Venture Capital</t>
-  </si>
-  <si>
-    <t>www.brightstonevc.com</t>
-  </si>
-  <si>
-    <t>Brookstone Venture Capital</t>
-  </si>
-  <si>
-    <t>www.brookstoneventurecapital.com</t>
-  </si>
-  <si>
-    <t>Gambit Ventures</t>
-  </si>
-  <si>
-    <t>www.meetgambit.com</t>
-  </si>
-  <si>
-    <t>ParaFi Capital</t>
-  </si>
-  <si>
-    <t>www.parafi.capital</t>
-  </si>
-  <si>
-    <t>Stout Street Capital</t>
-  </si>
-  <si>
-    <t>www.stoutstreetcapital.com</t>
-  </si>
-  <si>
-    <t>Quiet Capital</t>
-  </si>
-  <si>
-    <t>www.quiet.com</t>
-  </si>
-  <si>
-    <t>Flourish Ventures</t>
-  </si>
-  <si>
-    <t>www.flourishventures.com</t>
-  </si>
-  <si>
-    <t>New Age Ventures</t>
-  </si>
-  <si>
-    <t>www.newageventures.net</t>
-  </si>
-  <si>
-    <t>RET Ventures</t>
-  </si>
-  <si>
-    <t>www.ret.vc</t>
-  </si>
-  <si>
-    <t>Resolute Ventures</t>
-  </si>
-  <si>
-    <t>www.resolute.vc</t>
   </si>
 </sst>
 </file>
@@ -212,7 +122,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -230,6 +140,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -495,11 +409,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -583,126 +495,6 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>